<commit_message>
Wed Mar 26 06:50:04 AM CST 2025
</commit_message>
<xml_diff>
--- a/bosai/summary_month_2025_3/summary_month.xlsx
+++ b/bosai/summary_month_2025_3/summary_month.xlsx
@@ -1,18 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
     <workbookView windowWidth="28800" windowHeight="11355"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$30</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>项目部月报   __生信_ 部 黄礼闯   本月工作完成情况</t>
   </si>
@@ -62,99 +61,6 @@
     <t>备注/遇到问题</t>
   </si>
   <si>
-    <t>BS.develop</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>模块开发</t>
-  </si>
-  <si>
-    <t>诊断模型的多数据集构建和验证</t>
-  </si>
-  <si>
-    <t>用于快速操作多个数据集的诊断模型构建和验证</t>
-  </si>
-  <si>
-    <t>BS.eval</t>
-  </si>
-  <si>
-    <t>生信评估</t>
-  </si>
-  <si>
-    <t>血竭治疗压力性损伤网药及分子对接</t>
-  </si>
-  <si>
-    <t>scRNA-seq 细胞注释后自动绘制验证热图</t>
-  </si>
-  <si>
-    <t>智能挑选 CellMarker 数据库的特异性 Marker</t>
-  </si>
-  <si>
-    <t>BSCL250222</t>
-  </si>
-  <si>
-    <t>汪光亮</t>
-  </si>
-  <si>
-    <t>生信分析</t>
-  </si>
-  <si>
-    <t>MYLK分子对接</t>
-  </si>
-  <si>
-    <t>BSLL250310</t>
-  </si>
-  <si>
-    <t>马佩芬</t>
-  </si>
-  <si>
-    <t>思路设计</t>
-  </si>
-  <si>
-    <t>糖尿病创面</t>
-  </si>
-  <si>
-    <t>BSXG250226</t>
-  </si>
-  <si>
-    <t>公司内部</t>
-  </si>
-  <si>
-    <t>小鼠结肠炎的单细胞测序数据</t>
-  </si>
-  <si>
-    <t>BSJF211201</t>
-  </si>
-  <si>
-    <t>陶磊磊</t>
-  </si>
-  <si>
-    <t>补充分析</t>
-  </si>
-  <si>
-    <t>分子对接二氢杨梅素与ATF4</t>
-  </si>
-  <si>
-    <t>BSLL250203</t>
-  </si>
-  <si>
-    <t>王东敏</t>
-  </si>
-  <si>
-    <t>网药分析-单味药血竭</t>
-  </si>
-  <si>
-    <t>网药分析-复方</t>
-  </si>
-  <si>
-    <t>图片调整</t>
-  </si>
-  <si>
-    <t>饼图2和韦恩图4</t>
-  </si>
-  <si>
     <t>需协调与帮助：暂无</t>
   </si>
   <si>
@@ -170,7 +76,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
@@ -196,24 +102,28 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
       <charset val="0"/>
     </font>
     <font>
       <b/>
       <sz val="16"/>
       <name val="Microsoft YaHei"/>
+      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <name val="Microsoft YaHei"/>
+      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
       <charset val="0"/>
     </font>
     <font>
@@ -236,6 +146,7 @@
     <font>
       <sz val="14"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
       <charset val="0"/>
     </font>
     <font>
@@ -248,11 +159,13 @@
     <font>
       <sz val="10"/>
       <name val="Microsoft YaHei"/>
+      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
       <charset val="0"/>
     </font>
     <font>
@@ -263,6 +176,7 @@
     <font>
       <sz val="11"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
       <charset val="0"/>
     </font>
     <font>
@@ -935,7 +849,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -978,12 +892,18 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1005,8 +925,17 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
@@ -1014,10 +943,19 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="3" fillId="0" fontId="9" numFmtId="14" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="3" fillId="0" fontId="7" numFmtId="14" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1548,22 +1486,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <sheetPr/>
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="3" width="13.6285714285714" customWidth="1"/>
-    <col min="4" max="4" width="16.5714285714286" customWidth="1"/>
-    <col min="5" max="9" width="13.6285714285714" customWidth="1"/>
+    <col min="1" max="9" width="13.6285714285714" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="22.5" spans="1:9">
+    <row ht="22.5" r="1" spans="1:9">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1574,9 +1510,9 @@
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
-      <c r="I1" s="21"/>
-    </row>
-    <row r="2" ht="33" spans="1:9">
+      <c r="I1" s="23"/>
+    </row>
+    <row ht="33" r="2" spans="1:9">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -1605,509 +1541,691 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="1" ht="16.5" customHeight="1" spans="1:10">
-      <c r="A3" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="18">
+    <row customFormat="1" customHeight="1" ht="16.5" r="3" s="1" spans="1:9">
+      <c r="A3" s="7" t="inlineStr">
+        <is>
+          <t>BS.develop</t>
+        </is>
+      </c>
+      <c r="B3" s="8" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="C3" s="9" t="inlineStr">
+        <is>
+          <t>模块开发</t>
+        </is>
+      </c>
+      <c r="D3" s="8" t="inlineStr">
+        <is>
+          <t>诊断模型的多数据集构建和验证</t>
+        </is>
+      </c>
+      <c r="E3" s="34">
         <v>45715</v>
       </c>
-      <c r="F3" s="18">
+      <c r="F3" s="34">
         <v>45720</v>
       </c>
-      <c r="G3" s="18">
+      <c r="G3" s="34">
         <v>45720</v>
       </c>
-      <c r="H3" s="19">
+      <c r="H3" s="35">
         <v>45720</v>
       </c>
-      <c r="I3" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" s="1" customFormat="1" ht="16.5" customHeight="1" spans="1:10">
-      <c r="A4" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="18">
+      <c r="I3" s="24" t="inlineStr">
+        <is>
+          <t>用于快速操作多个数据集的诊断模型构建和验证</t>
+        </is>
+      </c>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="4" s="1" spans="1:9">
+      <c r="A4" s="7" t="inlineStr">
+        <is>
+          <t>BS.eval</t>
+        </is>
+      </c>
+      <c r="B4" s="10" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="C4" s="9" t="inlineStr">
+        <is>
+          <t>生信评估</t>
+        </is>
+      </c>
+      <c r="D4" s="10" t="inlineStr">
+        <is>
+          <t>血竭治疗压力性损伤网药及分子对接</t>
+        </is>
+      </c>
+      <c r="E4" s="34">
         <v>45721</v>
       </c>
-      <c r="F4" s="18">
+      <c r="F4" s="34">
         <v>45721</v>
       </c>
-      <c r="G4" s="18">
+      <c r="G4" s="34">
         <v>45721</v>
       </c>
-      <c r="H4" s="18">
+      <c r="H4" s="34">
         <v>45721</v>
       </c>
-      <c r="I4" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="J4" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" s="1" customFormat="1" ht="16.5" customHeight="1" spans="1:10">
-      <c r="A5" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="18">
+      <c r="I4" s="24" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="5" s="1" spans="1:9">
+      <c r="A5" s="7" t="inlineStr">
+        <is>
+          <t>BS.develop</t>
+        </is>
+      </c>
+      <c r="B5" s="7" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="C5" s="7" t="inlineStr">
+        <is>
+          <t>模块开发</t>
+        </is>
+      </c>
+      <c r="D5" s="10" t="inlineStr">
+        <is>
+          <t>scRNA-seq 细胞注释后自动绘制验证热图</t>
+        </is>
+      </c>
+      <c r="E5" s="34">
         <v>45722</v>
       </c>
-      <c r="F5" s="18">
+      <c r="F5" s="34">
         <v>45723</v>
       </c>
-      <c r="G5" s="18">
+      <c r="G5" s="34">
         <v>45723</v>
       </c>
-      <c r="H5" s="18">
+      <c r="H5" s="34">
         <v>45723</v>
       </c>
-      <c r="I5" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="J5" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" s="1" customFormat="1" ht="16.5" customHeight="1" spans="1:10">
-      <c r="A6" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="18">
+      <c r="I5" s="24" t="inlineStr">
+        <is>
+          <t>智能挑选 CellMarker 数据库的特异性 Marker</t>
+        </is>
+      </c>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="6" s="1" spans="1:9">
+      <c r="A6" s="7" t="inlineStr">
+        <is>
+          <t>BSCL250222</t>
+        </is>
+      </c>
+      <c r="B6" s="7" t="inlineStr">
+        <is>
+          <t>汪光亮</t>
+        </is>
+      </c>
+      <c r="C6" s="7" t="inlineStr">
+        <is>
+          <t>生信分析</t>
+        </is>
+      </c>
+      <c r="D6" s="7" t="inlineStr">
+        <is>
+          <t>MYLK分子对接</t>
+        </is>
+      </c>
+      <c r="E6" s="34">
         <v>45715</v>
       </c>
-      <c r="F6" s="18">
+      <c r="F6" s="34">
         <v>45721</v>
       </c>
-      <c r="G6" s="18">
+      <c r="G6" s="34">
         <v>45728</v>
       </c>
-      <c r="H6" s="18">
+      <c r="H6" s="34">
         <v>45728</v>
       </c>
-      <c r="I6" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="J6" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" s="1" customFormat="1" ht="16.5" customHeight="1" spans="1:10">
-      <c r="A7" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="18">
+      <c r="I6" s="24" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="7" s="1" spans="1:9">
+      <c r="A7" s="7" t="inlineStr">
+        <is>
+          <t>BSLL250310</t>
+        </is>
+      </c>
+      <c r="B7" s="7" t="inlineStr">
+        <is>
+          <t>马佩芬</t>
+        </is>
+      </c>
+      <c r="C7" s="11" t="inlineStr">
+        <is>
+          <t>思路设计</t>
+        </is>
+      </c>
+      <c r="D7" s="7" t="inlineStr">
+        <is>
+          <t>糖尿病创面</t>
+        </is>
+      </c>
+      <c r="E7" s="34">
         <v>45723</v>
       </c>
-      <c r="F7" s="18">
+      <c r="F7" s="34">
         <v>45730</v>
       </c>
-      <c r="G7" s="18">
+      <c r="G7" s="34">
         <v>45729</v>
       </c>
-      <c r="H7" s="18">
+      <c r="H7" s="34">
         <v>45729</v>
       </c>
-      <c r="I7" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="J7" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" s="1" customFormat="1" ht="16.5" customHeight="1" spans="1:10">
-      <c r="A8" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" s="18">
+      <c r="I7" s="24" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="8" s="1" spans="1:9">
+      <c r="A8" s="7" t="inlineStr">
+        <is>
+          <t>BSXG250226</t>
+        </is>
+      </c>
+      <c r="B8" s="7" t="inlineStr">
+        <is>
+          <t>公司内部</t>
+        </is>
+      </c>
+      <c r="C8" s="7" t="inlineStr">
+        <is>
+          <t>思路设计</t>
+        </is>
+      </c>
+      <c r="D8" s="7" t="inlineStr">
+        <is>
+          <t>小鼠结肠炎的单细胞测序数据</t>
+        </is>
+      </c>
+      <c r="E8" s="34">
         <v>45715</v>
       </c>
-      <c r="F8" s="18">
+      <c r="F8" s="34">
         <v>45726</v>
       </c>
-      <c r="G8" s="18">
+      <c r="G8" s="34">
         <v>45733</v>
       </c>
-      <c r="H8" s="18">
+      <c r="H8" s="34">
         <v>45733</v>
       </c>
-      <c r="I8" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="J8" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" s="1" customFormat="1" ht="16.5" customHeight="1" spans="1:10">
-      <c r="A9" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" s="18">
+      <c r="I8" s="24" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="9" s="1" spans="1:9">
+      <c r="A9" s="7" t="inlineStr">
+        <is>
+          <t>BSJF211201</t>
+        </is>
+      </c>
+      <c r="B9" s="7" t="inlineStr">
+        <is>
+          <t>陶磊磊</t>
+        </is>
+      </c>
+      <c r="C9" s="7" t="inlineStr">
+        <is>
+          <t>补充分析</t>
+        </is>
+      </c>
+      <c r="D9" s="7" t="inlineStr">
+        <is>
+          <t>分子对接二氢杨梅素与ATF4</t>
+        </is>
+      </c>
+      <c r="E9" s="34">
         <v>45379</v>
       </c>
-      <c r="F9" s="18">
+      <c r="F9" s="34">
         <v>45734</v>
       </c>
-      <c r="G9" s="18">
+      <c r="G9" s="34">
         <v>45734</v>
       </c>
-      <c r="H9" s="18">
+      <c r="H9" s="34">
         <v>45734</v>
       </c>
-      <c r="I9" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="J9" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" s="2" customFormat="1" ht="16.5" customHeight="1" spans="1:10">
-      <c r="A10" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10" s="18">
+      <c r="I9" s="24" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="10" s="2" spans="1:9">
+      <c r="A10" s="7" t="inlineStr">
+        <is>
+          <t>BSLL250203</t>
+        </is>
+      </c>
+      <c r="B10" s="7" t="inlineStr">
+        <is>
+          <t>王东敏</t>
+        </is>
+      </c>
+      <c r="C10" s="11" t="inlineStr">
+        <is>
+          <t>生信分析</t>
+        </is>
+      </c>
+      <c r="D10" s="7" t="inlineStr">
+        <is>
+          <t>网药分析-单味药血竭</t>
+        </is>
+      </c>
+      <c r="E10" s="34">
         <v>45702</v>
       </c>
-      <c r="F10" s="18">
+      <c r="F10" s="34">
         <v>45730</v>
       </c>
-      <c r="G10" s="18">
+      <c r="G10" s="34">
         <v>45729</v>
       </c>
-      <c r="H10" s="18">
+      <c r="H10" s="34">
         <v>45729</v>
       </c>
-      <c r="I10" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="J10" s="2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" s="1" customFormat="1" ht="16.5" customHeight="1" spans="1:10">
-      <c r="A11" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E11" s="18">
+      <c r="I10" s="25" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="11" s="1" spans="1:9">
+      <c r="A11" s="7" t="inlineStr">
+        <is>
+          <t>BSLL250203</t>
+        </is>
+      </c>
+      <c r="B11" s="12" t="inlineStr">
+        <is>
+          <t>王东敏</t>
+        </is>
+      </c>
+      <c r="C11" s="7" t="inlineStr">
+        <is>
+          <t>生信分析</t>
+        </is>
+      </c>
+      <c r="D11" s="7" t="inlineStr">
+        <is>
+          <t>网药分析-复方</t>
+        </is>
+      </c>
+      <c r="E11" s="34">
         <v>45702</v>
       </c>
-      <c r="F11" s="18">
+      <c r="F11" s="34">
         <v>45730</v>
       </c>
-      <c r="G11" s="18">
+      <c r="G11" s="34">
         <v>45729</v>
       </c>
-      <c r="H11" s="18">
+      <c r="H11" s="34">
         <v>45729</v>
       </c>
-      <c r="I11" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="J11" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" ht="18" spans="1:10">
-      <c r="A12" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E12" s="18">
+      <c r="I11" s="26" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row ht="18" r="12" spans="1:9">
+      <c r="A12" s="7" t="inlineStr">
+        <is>
+          <t>BSLL250203</t>
+        </is>
+      </c>
+      <c r="B12" s="7" t="inlineStr">
+        <is>
+          <t>王东敏</t>
+        </is>
+      </c>
+      <c r="C12" s="7" t="inlineStr">
+        <is>
+          <t>补充分析</t>
+        </is>
+      </c>
+      <c r="D12" s="7" t="inlineStr">
+        <is>
+          <t>图片调整</t>
+        </is>
+      </c>
+      <c r="E12" s="34">
         <v>45336</v>
       </c>
-      <c r="F12" s="18">
+      <c r="F12" s="34">
         <v>45734</v>
       </c>
-      <c r="G12" s="18">
+      <c r="G12" s="34">
         <v>45735</v>
       </c>
-      <c r="H12" s="18">
+      <c r="H12" s="34">
         <v>45735</v>
       </c>
-      <c r="I12" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="J12">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" s="1" customFormat="1" ht="16.5" customHeight="1" spans="1:9">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="22"/>
-    </row>
-    <row r="14" s="1" customFormat="1" ht="16.5" customHeight="1" spans="1:9">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="22"/>
-    </row>
-    <row r="15" s="1" customFormat="1" ht="16.5" customHeight="1" spans="1:9">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="22"/>
-    </row>
-    <row r="16" ht="18" spans="1:9">
-      <c r="A16" s="13"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="24"/>
-    </row>
-    <row r="17" s="1" customFormat="1" ht="16.5" customHeight="1" spans="1:9">
+      <c r="I12" s="27" t="inlineStr">
+        <is>
+          <t>饼图2和韦恩图4</t>
+        </is>
+      </c>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="13" s="1" spans="1:9">
+      <c r="A13" s="7" t="inlineStr">
+        <is>
+          <t>BS.develop</t>
+        </is>
+      </c>
+      <c r="B13" s="7" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="C13" s="7" t="inlineStr">
+        <is>
+          <t>模块开发</t>
+        </is>
+      </c>
+      <c r="D13" s="7" t="inlineStr">
+        <is>
+          <t>增强 GEO 检测策略</t>
+        </is>
+      </c>
+      <c r="E13" s="34">
+        <v>45737</v>
+      </c>
+      <c r="F13" s="34">
+        <v>45737</v>
+      </c>
+      <c r="G13" s="34">
+        <v>45737</v>
+      </c>
+      <c r="H13" s="34">
+        <v>45737</v>
+      </c>
+      <c r="I13" s="26" t="inlineStr">
+        <is>
+          <t>抓取网页匹配 'Overall design' 和 'Sample' 名</t>
+        </is>
+      </c>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="14" s="1" spans="1:9">
+      <c r="A14" s="7" t="inlineStr">
+        <is>
+          <t>BSJF241107</t>
+        </is>
+      </c>
+      <c r="B14" s="7" t="inlineStr">
+        <is>
+          <t>许冠华</t>
+        </is>
+      </c>
+      <c r="C14" s="7" t="inlineStr">
+        <is>
+          <t>生信协助</t>
+        </is>
+      </c>
+      <c r="D14" s="12" t="inlineStr">
+        <is>
+          <t>脓毒症</t>
+        </is>
+      </c>
+      <c r="E14" s="34">
+        <v>45617</v>
+      </c>
+      <c r="F14" s="34">
+        <v>45737</v>
+      </c>
+      <c r="G14" s="34">
+        <v>45741</v>
+      </c>
+      <c r="H14" s="34">
+        <v>45741</v>
+      </c>
+      <c r="I14" s="28" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="15" s="1" spans="1:9">
+      <c r="A15" s="7" t="inlineStr">
+        <is>
+          <t>BSXN240936</t>
+        </is>
+      </c>
+      <c r="B15" s="7" t="inlineStr">
+        <is>
+          <t>李扬</t>
+        </is>
+      </c>
+      <c r="C15" s="7" t="inlineStr">
+        <is>
+          <t>生信协助</t>
+        </is>
+      </c>
+      <c r="D15" s="12" t="inlineStr">
+        <is>
+          <t>补充 METTL</t>
+        </is>
+      </c>
+      <c r="E15" s="34">
+        <v>45562</v>
+      </c>
+      <c r="F15" s="34">
+        <v>45742</v>
+      </c>
+      <c r="G15" s="34">
+        <v>45741</v>
+      </c>
+      <c r="H15" s="34">
+        <v>45741</v>
+      </c>
+      <c r="I15" s="28" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row ht="18" r="16" spans="1:9">
+      <c r="A16" s="13" t="inlineStr">
+        <is>
+          <t>BSJF240124</t>
+        </is>
+      </c>
+      <c r="B16" s="13" t="inlineStr">
+        <is>
+          <t>蒋镥</t>
+        </is>
+      </c>
+      <c r="C16" s="13" t="inlineStr">
+        <is>
+          <t>生信协助</t>
+        </is>
+      </c>
+      <c r="D16" s="13" t="inlineStr">
+        <is>
+          <t>预测结合转录子</t>
+        </is>
+      </c>
+      <c r="E16" s="34">
+        <v>45534</v>
+      </c>
+      <c r="F16" s="34">
+        <v>45740</v>
+      </c>
+      <c r="G16" s="34">
+        <v>45741</v>
+      </c>
+      <c r="H16" s="34">
+        <v>45741</v>
+      </c>
+      <c r="I16" s="29" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="17" s="1" spans="1:9">
       <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
+      <c r="B17" s="14"/>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="25"/>
-    </row>
-    <row r="18" s="1" customFormat="1" ht="16.5" customHeight="1" spans="1:9">
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="30"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="18" s="1" spans="1:9">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="25"/>
-    </row>
-    <row r="19" s="1" customFormat="1" ht="16.5" customHeight="1" spans="1:9">
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="30"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="19" s="1" spans="1:9">
       <c r="A19" s="7"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="25"/>
-    </row>
-    <row r="20" s="1" customFormat="1" ht="16.5" customHeight="1" spans="1:9">
-      <c r="A20" s="14"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="25"/>
-    </row>
-    <row r="21" s="1" customFormat="1" ht="16.5" customHeight="1" spans="1:9">
-      <c r="A21" s="14"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18"/>
-      <c r="I21" s="25"/>
-    </row>
-    <row r="22" customFormat="1" spans="1:9">
-      <c r="A22" s="15"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="26"/>
-    </row>
-    <row r="23" customFormat="1" spans="1:9">
-      <c r="A23" s="15"/>
-      <c r="B23" s="15"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="15"/>
-      <c r="I23" s="26"/>
-    </row>
-    <row r="24" customFormat="1" spans="1:9">
-      <c r="A24" s="15"/>
-      <c r="B24" s="15"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
-      <c r="I24" s="26"/>
-    </row>
-    <row r="25" customFormat="1" spans="1:9">
-      <c r="A25" s="15"/>
-      <c r="B25" s="15"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="15"/>
-      <c r="I25" s="26"/>
-    </row>
-    <row r="26" customFormat="1" spans="1:9">
-      <c r="A26" s="15"/>
-      <c r="B26" s="15"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="15"/>
-      <c r="I26" s="26"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="30"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="20" s="1" spans="1:9">
+      <c r="A20" s="15"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="30"/>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="21" s="1" spans="1:9">
+      <c r="A21" s="15"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="31"/>
+    </row>
+    <row customFormat="1" r="22" spans="1:9">
+      <c r="A22" s="16"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="32"/>
+    </row>
+    <row customFormat="1" r="23" spans="1:9">
+      <c r="A23" s="16"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="32"/>
+    </row>
+    <row customFormat="1" r="24" spans="1:9">
+      <c r="A24" s="16"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="32"/>
+    </row>
+    <row customFormat="1" r="25" spans="1:9">
+      <c r="A25" s="16"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="32"/>
+    </row>
+    <row customFormat="1" r="26" spans="1:9">
+      <c r="A26" s="16"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="32"/>
     </row>
     <row r="27" spans="1:9">
-      <c r="A27" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="B27" s="15"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="15"/>
-      <c r="I27" s="15"/>
+      <c r="A27" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="17"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="17"/>
     </row>
     <row r="28" spans="1:9">
-      <c r="A28" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="B28" s="15"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="15"/>
-      <c r="I28" s="15"/>
-    </row>
-    <row r="29" ht="22.5" spans="1:9">
+      <c r="A28" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="17"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="17"/>
+      <c r="I28" s="17"/>
+    </row>
+    <row ht="22.5" r="29" spans="1:9">
       <c r="A29" s="4" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -2116,9 +2234,9 @@
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
-      <c r="I29" s="21"/>
-    </row>
-    <row r="30" ht="33" spans="1:9">
+      <c r="I29" s="23"/>
+    </row>
+    <row ht="33" r="30" spans="1:9">
       <c r="A30" s="6" t="s">
         <v>1</v>
       </c>
@@ -2147,51 +2265,51 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" ht="16.5" customHeight="1" spans="1:9">
-      <c r="A31" s="16"/>
-      <c r="B31" s="17"/>
-      <c r="C31" s="17"/>
-      <c r="D31" s="17"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="20"/>
-      <c r="H31" s="20"/>
-      <c r="I31" s="27"/>
-    </row>
-    <row r="32" s="3" customFormat="1" spans="1:9">
-      <c r="A32" s="16"/>
-      <c r="B32" s="16"/>
-      <c r="C32" s="16"/>
-      <c r="D32" s="16"/>
-      <c r="E32" s="20"/>
-      <c r="F32" s="20"/>
-      <c r="G32" s="20"/>
-      <c r="H32" s="20"/>
-      <c r="I32" s="16"/>
+    <row customHeight="1" ht="16.5" r="31" spans="1:9">
+      <c r="A31" s="18"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="22"/>
+      <c r="I31" s="33"/>
+    </row>
+    <row customFormat="1" r="32" s="3" spans="1:9">
+      <c r="A32" s="18"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="22"/>
+      <c r="H32" s="22"/>
+      <c r="I32" s="18"/>
     </row>
     <row r="33" spans="1:9">
-      <c r="A33" s="17"/>
-      <c r="B33" s="17"/>
-      <c r="C33" s="17"/>
-      <c r="D33" s="17"/>
-      <c r="E33" s="17"/>
-      <c r="F33" s="17"/>
-      <c r="G33" s="17"/>
-      <c r="H33" s="17"/>
-      <c r="I33" s="17"/>
-    </row>
-    <row r="34" ht="28.5" spans="1:9">
-      <c r="A34" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="B34" s="15"/>
-      <c r="C34" s="15"/>
-      <c r="D34" s="15"/>
-      <c r="E34" s="15"/>
-      <c r="F34" s="15"/>
-      <c r="G34" s="15"/>
-      <c r="H34" s="15"/>
-      <c r="I34" s="17"/>
+      <c r="A33" s="19"/>
+      <c r="B33" s="19"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="19"/>
+      <c r="H33" s="19"/>
+      <c r="I33" s="19"/>
+    </row>
+    <row ht="28.5" r="34" spans="1:9">
+      <c r="A34" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" s="17"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="17"/>
+      <c r="H34" s="17"/>
+      <c r="I34" s="19"/>
     </row>
   </sheetData>
   <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:I30" etc:filterBottomFollowUsedRange="0">
@@ -2204,6 +2322,5 @@
     <mergeCell ref="A29:I29"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fri Mar 28 06:50:05 AM CST 2025
</commit_message>
<xml_diff>
--- a/bosai/summary_month_2025_3/summary_month.xlsx
+++ b/bosai/summary_month_2025_3/summary_month.xlsx
@@ -2066,7 +2066,7 @@
       </c>
       <c r="D16" s="13" t="inlineStr">
         <is>
-          <t>预测结合转录子</t>
+          <t>结合转录因子</t>
         </is>
       </c>
       <c r="E16" s="34">
@@ -2076,10 +2076,10 @@
         <v>45740</v>
       </c>
       <c r="G16" s="34">
-        <v>45741</v>
+        <v>45743</v>
       </c>
       <c r="H16" s="34">
-        <v>45741</v>
+        <v>45743</v>
       </c>
       <c r="I16" s="29" t="inlineStr">
         <is>
@@ -2088,15 +2088,43 @@
       </c>
     </row>
     <row customFormat="1" customHeight="1" ht="16.5" r="17" s="1" spans="1:9">
-      <c r="A17" s="7"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="30"/>
+      <c r="A17" s="7" t="inlineStr">
+        <is>
+          <t>BS.develop</t>
+        </is>
+      </c>
+      <c r="B17" s="14" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="C17" s="7" t="inlineStr">
+        <is>
+          <t>模块开发</t>
+        </is>
+      </c>
+      <c r="D17" s="7" t="inlineStr">
+        <is>
+          <t>转录因子数据获取和可视化</t>
+        </is>
+      </c>
+      <c r="E17" s="34">
+        <v>45742</v>
+      </c>
+      <c r="F17" s="34">
+        <v>45743</v>
+      </c>
+      <c r="G17" s="34">
+        <v>45743</v>
+      </c>
+      <c r="H17" s="34">
+        <v>45743</v>
+      </c>
+      <c r="I17" s="30" t="inlineStr">
+        <is>
+          <t>抓取 hTFtarget 数据库程序，转录因子可视化程序</t>
+        </is>
+      </c>
     </row>
     <row customFormat="1" customHeight="1" ht="16.5" r="18" s="1" spans="1:9">
       <c r="A18" s="7"/>

</xml_diff>

<commit_message>
Sat Mar 29 06:50:04 AM CST 2025
</commit_message>
<xml_diff>
--- a/bosai/summary_month_2025_3/summary_month.xlsx
+++ b/bosai/summary_month_2025_3/summary_month.xlsx
@@ -2051,29 +2051,29 @@
     <row ht="18" r="16" spans="1:9">
       <c r="A16" s="13" t="inlineStr">
         <is>
-          <t>BSJF240124</t>
+          <t>BSHQ240813</t>
         </is>
       </c>
       <c r="B16" s="13" t="inlineStr">
         <is>
-          <t>蒋镥</t>
+          <t>王凯</t>
         </is>
       </c>
       <c r="C16" s="13" t="inlineStr">
         <is>
-          <t>生信协助</t>
+          <t>分析优化</t>
         </is>
       </c>
       <c r="D16" s="13" t="inlineStr">
         <is>
-          <t>结合转录因子</t>
+          <t>黑色素瘤</t>
         </is>
       </c>
       <c r="E16" s="34">
-        <v>45534</v>
+        <v>45743</v>
       </c>
       <c r="F16" s="34">
-        <v>45740</v>
+        <v>45744</v>
       </c>
       <c r="G16" s="34">
         <v>45743</v>
@@ -2090,29 +2090,29 @@
     <row customFormat="1" customHeight="1" ht="16.5" r="17" s="1" spans="1:9">
       <c r="A17" s="7" t="inlineStr">
         <is>
-          <t>BS.develop</t>
+          <t>BSJF240124</t>
         </is>
       </c>
       <c r="B17" s="14" t="inlineStr">
         <is>
-          <t/>
+          <t>蒋镥</t>
         </is>
       </c>
       <c r="C17" s="7" t="inlineStr">
         <is>
-          <t>模块开发</t>
+          <t>生信协助</t>
         </is>
       </c>
       <c r="D17" s="7" t="inlineStr">
         <is>
-          <t>转录因子数据获取和可视化</t>
+          <t>结合转录因子</t>
         </is>
       </c>
       <c r="E17" s="34">
-        <v>45742</v>
+        <v>45534</v>
       </c>
       <c r="F17" s="34">
-        <v>45743</v>
+        <v>45740</v>
       </c>
       <c r="G17" s="34">
         <v>45743</v>
@@ -2122,20 +2122,48 @@
       </c>
       <c r="I17" s="30" t="inlineStr">
         <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row customFormat="1" customHeight="1" ht="16.5" r="18" s="1" spans="1:9">
+      <c r="A18" s="7" t="inlineStr">
+        <is>
+          <t>BS.develop</t>
+        </is>
+      </c>
+      <c r="B18" s="7" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="C18" s="7" t="inlineStr">
+        <is>
+          <t>模块开发</t>
+        </is>
+      </c>
+      <c r="D18" s="7" t="inlineStr">
+        <is>
+          <t>转录因子数据获取和可视化</t>
+        </is>
+      </c>
+      <c r="E18" s="34">
+        <v>45742</v>
+      </c>
+      <c r="F18" s="34">
+        <v>45743</v>
+      </c>
+      <c r="G18" s="34">
+        <v>45743</v>
+      </c>
+      <c r="H18" s="34">
+        <v>45743</v>
+      </c>
+      <c r="I18" s="30" t="inlineStr">
+        <is>
           <t>抓取 hTFtarget 数据库程序，转录因子可视化程序</t>
         </is>
       </c>
-    </row>
-    <row customFormat="1" customHeight="1" ht="16.5" r="18" s="1" spans="1:9">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="30"/>
     </row>
     <row customFormat="1" customHeight="1" ht="16.5" r="19" s="1" spans="1:9">
       <c r="A19" s="7"/>

</xml_diff>